<commit_message>
Fix: Property csvEncoding of xava.properties has no effect when importing CSV files
</commit_message>
<xml_diff>
--- a/openxavatest/test-files/appointments.xlsx
+++ b/openxavatest/test-files/appointments.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Driving my BMW</t>
   </si>
   <si>
-    <t xml:space="preserve">Playing Fortnite</t>
+    <t xml:space="preserve">Playing Fórtnite</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
@@ -67,7 +67,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YY\ H:MM\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm\ AM/PM"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -167,23 +167,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="30.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -272,8 +271,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>